<commit_message>
intel updated and added quarters
</commit_message>
<xml_diff>
--- a/intc.xlsx
+++ b/intc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13099D0E-3555-4643-9637-6FFF6065A199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245DE2B1-2E47-4F33-A253-572799D5E667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="0" windowWidth="24075" windowHeight="20985" activeTab="1" xr2:uid="{CA272A53-6244-429C-A241-B4996EB13F3D}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{CA272A53-6244-429C-A241-B4996EB13F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t>Intel Corp</t>
   </si>
@@ -420,9 +420,6 @@
     <t>q123</t>
   </si>
   <si>
-    <t>Q224</t>
-  </si>
-  <si>
     <t>q422</t>
   </si>
   <si>
@@ -451,6 +448,30 @@
   </si>
   <si>
     <t>check these #</t>
+  </si>
+  <si>
+    <t>q324</t>
+  </si>
+  <si>
+    <t>16,500 headcount reduction</t>
+  </si>
+  <si>
+    <t>awarded up to $3B in direct funding under CHIPS and Science Act</t>
+  </si>
+  <si>
+    <t>launched latest of x86 processors, the Intel Core Ultra 200V series processors</t>
+  </si>
+  <si>
+    <t>announced next gen of AI solutoins with the launch of Intel Xeon 6 processor with Performance-cores and the Intel Gaudi 3 AI accelerator</t>
+  </si>
+  <si>
+    <t>op cash flow</t>
+  </si>
+  <si>
+    <t>capex</t>
+  </si>
+  <si>
+    <t>fcf</t>
   </si>
 </sst>
 </file>
@@ -504,12 +525,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -518,7 +548,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -530,6 +560,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -866,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83573467-9CE6-46BC-A3D1-C5F0D3921F38}">
-  <dimension ref="B1:M102"/>
+  <dimension ref="B1:M110"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>18.89</v>
+        <v>24.84</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -912,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="L5" s="3">
-        <v>4276</v>
+        <v>4313</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -927,7 +959,7 @@
       </c>
       <c r="L6">
         <f>L5*L4</f>
-        <v>80773.64</v>
+        <v>107134.92</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -939,11 +971,11 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <f>11287+17986</f>
-        <v>29273</v>
+        <f>8785+15301</f>
+        <v>24086</v>
       </c>
       <c r="M7" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -951,10 +983,11 @@
         <v>5</v>
       </c>
       <c r="L8">
-        <v>48334</v>
+        <f>35159</f>
+        <v>35159</v>
       </c>
       <c r="M8" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -963,7 +996,7 @@
       </c>
       <c r="L9">
         <f>L6+L8-L7</f>
-        <v>99834.64</v>
+        <v>118207.91999999998</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -1347,34 +1380,59 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1384,41 +1442,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B64B1D-20CF-45BB-8B2C-E1E075C773C3}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="O12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
         <v>126</v>
@@ -1438,23 +1497,26 @@
       <c r="L2" t="s">
         <v>121</v>
       </c>
-      <c r="N2">
+      <c r="M2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2">
         <v>2021</v>
       </c>
-      <c r="O2">
-        <f t="shared" ref="O2:Q2" si="0">N2+1</f>
+      <c r="Q2">
+        <f t="shared" ref="Q2:S2" si="0">P2+1</f>
         <v>2022</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>97</v>
       </c>
@@ -1470,19 +1532,22 @@
       <c r="L3">
         <v>4480</v>
       </c>
-      <c r="N3" s="3">
-        <f>O3+6700</f>
+      <c r="M3">
+        <v>4888</v>
+      </c>
+      <c r="P3" s="3">
+        <f>Q3+6700</f>
         <v>25500</v>
       </c>
-      <c r="O3" s="3">
-        <f>P3+1800</f>
+      <c r="Q3" s="3">
+        <f>R3+1800</f>
         <v>18800</v>
       </c>
-      <c r="P3" s="3">
+      <c r="R3" s="3">
         <v>17000</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>98</v>
       </c>
@@ -1498,19 +1563,22 @@
       <c r="L4">
         <v>2527</v>
       </c>
-      <c r="N4" s="3">
-        <f>O4+1800</f>
+      <c r="M4">
+        <v>2070</v>
+      </c>
+      <c r="P4" s="3">
+        <f>Q4+1800</f>
         <v>12495</v>
       </c>
-      <c r="O4" s="3">
-        <f>P4+495</f>
+      <c r="Q4" s="3">
+        <f>R4+495</f>
         <v>10695</v>
       </c>
-      <c r="P4" s="3">
+      <c r="R4" s="3">
         <v>10200</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>99</v>
       </c>
@@ -1526,21 +1594,24 @@
       <c r="L5">
         <v>403</v>
       </c>
-      <c r="N5" s="3">
-        <f>O5+870</f>
+      <c r="M5">
+        <v>372</v>
+      </c>
+      <c r="P5" s="3">
+        <f>Q5+870</f>
         <v>3199</v>
       </c>
-      <c r="O5" s="3">
-        <f>P5+229</f>
+      <c r="Q5" s="3">
+        <f>R5+229</f>
         <v>2329</v>
       </c>
-      <c r="P5" s="3">
+      <c r="R5" s="3">
         <v>2100</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6">
         <v>4255</v>
@@ -1554,13 +1625,16 @@
       <c r="L6">
         <v>3045</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="M6">
+        <v>3349</v>
+      </c>
       <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7">
         <v>2133</v>
@@ -1574,13 +1648,16 @@
       <c r="L7">
         <v>1344</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="M7">
+        <v>1511</v>
+      </c>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8">
         <v>450</v>
@@ -1594,16 +1671,19 @@
       <c r="L8">
         <v>440</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="M8">
+        <v>485</v>
+      </c>
       <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9">
         <v>78</v>
@@ -1617,13 +1697,16 @@
       <c r="L9" s="5">
         <v>4320</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="M9" s="5">
+        <v>4352</v>
+      </c>
       <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10">
         <v>294</v>
@@ -1635,16 +1718,20 @@
         <f>968-L8</f>
         <v>528</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="M10">
+        <f>142+412</f>
+        <v>554</v>
+      </c>
       <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P11" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>101</v>
       </c>
@@ -1659,7 +1746,7 @@
         <v>14158</v>
       </c>
       <c r="J13" s="3">
-        <f>(P13-(SUM(G13:I13)))</f>
+        <f>(R13-(SUM(G13:I13)))</f>
         <v>15406</v>
       </c>
       <c r="K13" s="6">
@@ -1669,17 +1756,20 @@
       <c r="L13" s="6">
         <v>12833</v>
       </c>
-      <c r="N13" s="3">
+      <c r="M13" s="6">
+        <v>13284</v>
+      </c>
+      <c r="P13" s="3">
         <v>79024</v>
       </c>
-      <c r="O13" s="3">
+      <c r="Q13" s="3">
         <v>63054</v>
       </c>
-      <c r="P13" s="3">
+      <c r="R13" s="3">
         <v>54228</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>102</v>
       </c>
@@ -1693,7 +1783,7 @@
         <v>-8140</v>
       </c>
       <c r="J14" s="6">
-        <f>P14-SUM(G14:I14)</f>
+        <f>R14-SUM(G14:I14)</f>
         <v>-8359</v>
       </c>
       <c r="K14" s="6">
@@ -1702,18 +1792,21 @@
       <c r="L14" s="6">
         <v>-8286</v>
       </c>
-      <c r="N14" s="6">
+      <c r="M14" s="6">
+        <v>-11287</v>
+      </c>
+      <c r="P14" s="6">
         <v>-35209</v>
       </c>
-      <c r="O14" s="6">
+      <c r="Q14" s="6">
         <v>-36188</v>
       </c>
-      <c r="P14" s="6">
+      <c r="R14" s="6">
         <v>-32517</v>
       </c>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>103</v>
       </c>
@@ -1741,20 +1834,24 @@
         <f t="shared" si="1"/>
         <v>4547</v>
       </c>
-      <c r="N15" s="7">
-        <f>SUM(N13,N14)</f>
+      <c r="M15" s="10">
+        <f t="shared" ref="M15" si="2">SUM(M13:M14)</f>
+        <v>1997</v>
+      </c>
+      <c r="P15" s="7">
+        <f>SUM(P13,P14)</f>
         <v>43815</v>
       </c>
-      <c r="O15" s="7">
-        <f t="shared" ref="O15:P15" si="2">SUM(O13,O14)</f>
+      <c r="Q15" s="7">
+        <f t="shared" ref="Q15:R15" si="3">SUM(Q13,Q14)</f>
         <v>26866</v>
       </c>
-      <c r="P15" s="7">
-        <f t="shared" si="2"/>
+      <c r="R15" s="7">
+        <f t="shared" si="3"/>
         <v>21711</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>104</v>
       </c>
@@ -1768,7 +1865,7 @@
         <v>-3870</v>
       </c>
       <c r="J16" s="6">
-        <f>P16-SUM(G16:I16)</f>
+        <f>R16-SUM(G16:I16)</f>
         <v>-3987</v>
       </c>
       <c r="K16" s="6">
@@ -1777,17 +1874,20 @@
       <c r="L16" s="6">
         <v>-4239</v>
       </c>
-      <c r="N16" s="6">
+      <c r="M16" s="6">
+        <v>-4049</v>
+      </c>
+      <c r="P16" s="6">
         <v>-15190</v>
       </c>
-      <c r="O16" s="6">
+      <c r="Q16" s="6">
         <v>-17528</v>
       </c>
-      <c r="P16" s="6">
+      <c r="R16" s="6">
         <v>-16046</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>105</v>
       </c>
@@ -1801,7 +1901,7 @@
         <v>-1340</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" ref="J17:J18" si="3">P17-SUM(G17:I17)</f>
+        <f t="shared" ref="J17:J18" si="4">R17-SUM(G17:I17)</f>
         <v>-1617</v>
       </c>
       <c r="K17" s="6">
@@ -1810,17 +1910,20 @@
       <c r="L17" s="6">
         <v>-1329</v>
       </c>
-      <c r="N17" s="6">
+      <c r="M17" s="6">
+        <v>-1383</v>
+      </c>
+      <c r="P17" s="6">
         <v>-6543</v>
       </c>
-      <c r="O17" s="6">
+      <c r="Q17" s="6">
         <v>-7002</v>
       </c>
-      <c r="P17" s="6">
+      <c r="R17" s="6">
         <v>-5634</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>106</v>
       </c>
@@ -1834,7 +1937,7 @@
         <v>-816</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1142</v>
       </c>
       <c r="K18" s="6">
@@ -1843,17 +1946,20 @@
       <c r="L18" s="6">
         <v>-943</v>
       </c>
-      <c r="N18" s="6">
+      <c r="M18" s="6">
+        <v>-5622</v>
+      </c>
+      <c r="P18" s="6">
         <v>-2626</v>
       </c>
-      <c r="O18" s="6">
+      <c r="Q18" s="6">
         <v>-2</v>
       </c>
-      <c r="P18" s="6">
+      <c r="R18" s="6">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>107</v>
       </c>
@@ -1866,35 +1972,39 @@
         <v>-5654</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" ref="I19:L19" si="4">SUM(I16:I18)</f>
+        <f t="shared" ref="I19:L19" si="5">SUM(I16:I18)</f>
         <v>-6026</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-4462</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6286</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6511</v>
       </c>
-      <c r="N19" s="6">
-        <f>SUM(N16:N18)</f>
+      <c r="M19" s="6">
+        <f t="shared" ref="M19" si="6">SUM(M16:M18)</f>
+        <v>-11054</v>
+      </c>
+      <c r="P19" s="6">
+        <f>SUM(P16:P18)</f>
         <v>-24359</v>
       </c>
-      <c r="O19" s="6">
-        <f t="shared" ref="O19:P19" si="5">SUM(O16:O18)</f>
+      <c r="Q19" s="6">
+        <f t="shared" ref="Q19:R19" si="7">SUM(Q16:Q18)</f>
         <v>-24532</v>
       </c>
-      <c r="P19" s="6">
-        <f t="shared" si="5"/>
+      <c r="R19" s="6">
+        <f t="shared" si="7"/>
         <v>-21618</v>
       </c>
     </row>
-    <row r="20" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>108</v>
       </c>
@@ -1907,35 +2017,39 @@
         <v>-1016</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" ref="I20:L20" si="6">I15+I19</f>
+        <f t="shared" ref="I20:L20" si="8">I15+I19</f>
         <v>-8</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2585</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1069</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1964</v>
       </c>
-      <c r="N20" s="7">
-        <f>N15+N19</f>
+      <c r="M20" s="10">
+        <f t="shared" ref="M20" si="9">M15+M19</f>
+        <v>-9057</v>
+      </c>
+      <c r="P20" s="7">
+        <f>P15+P19</f>
         <v>19456</v>
       </c>
-      <c r="O20" s="7">
-        <f t="shared" ref="O20:P20" si="7">O15+O19</f>
+      <c r="Q20" s="7">
+        <f t="shared" ref="Q20:R20" si="10">Q15+Q19</f>
         <v>2334</v>
       </c>
-      <c r="P20" s="7">
-        <f t="shared" si="7"/>
+      <c r="R20" s="7">
+        <f t="shared" si="10"/>
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>109</v>
       </c>
@@ -1955,17 +2069,20 @@
       <c r="L21" s="6">
         <v>-120</v>
       </c>
-      <c r="N21" s="6">
+      <c r="M21" s="6">
+        <v>-159</v>
+      </c>
+      <c r="P21" s="6">
         <v>2729</v>
       </c>
-      <c r="O21" s="6">
+      <c r="Q21" s="6">
         <v>4268</v>
       </c>
-      <c r="P21" s="6">
+      <c r="R21" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -1985,17 +2102,20 @@
       <c r="L22" s="6">
         <v>80</v>
       </c>
-      <c r="N22" s="6">
+      <c r="M22" s="6">
+        <v>130</v>
+      </c>
+      <c r="P22" s="6">
         <v>-482</v>
       </c>
-      <c r="O22" s="6">
+      <c r="Q22" s="6">
         <v>1166</v>
       </c>
-      <c r="P22" s="6">
+      <c r="R22" s="6">
         <v>629</v>
       </c>
     </row>
-    <row r="23" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>111</v>
       </c>
@@ -2008,35 +2128,39 @@
         <v>-816</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" ref="I23:L23" si="8">SUM(I20:I22)</f>
+        <f t="shared" ref="I23:L23" si="11">SUM(I20:I22)</f>
         <v>-52</v>
       </c>
       <c r="J23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2585</v>
       </c>
       <c r="K23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-719</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-2004</v>
       </c>
-      <c r="N23" s="7">
-        <f>SUM(N20:N22)</f>
+      <c r="M23" s="6">
+        <f t="shared" ref="M23" si="12">SUM(M20:M22)</f>
+        <v>-9086</v>
+      </c>
+      <c r="P23" s="7">
+        <f>SUM(P20:P22)</f>
         <v>21703</v>
       </c>
-      <c r="O23" s="7">
-        <f t="shared" ref="O23:P23" si="9">SUM(O20:O22)</f>
+      <c r="Q23" s="7">
+        <f t="shared" ref="Q23:R23" si="13">SUM(Q20:Q22)</f>
         <v>7768</v>
       </c>
-      <c r="P23" s="7">
-        <f t="shared" si="9"/>
+      <c r="R23" s="7">
+        <f t="shared" si="13"/>
         <v>762</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>112</v>
       </c>
@@ -2056,20 +2180,20 @@
       <c r="L24" s="6">
         <v>350</v>
       </c>
-      <c r="N24" s="6">
+      <c r="M24" s="6">
+        <v>-7903</v>
+      </c>
+      <c r="P24" s="6">
         <v>-482</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>249</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <v>913</v>
       </c>
-      <c r="Q24">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>113</v>
       </c>
@@ -2082,253 +2206,296 @@
         <v>1473</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" ref="I25:L25" si="10">SUM(I23:I24)</f>
+        <f t="shared" ref="I25:L25" si="14">SUM(I23:I24)</f>
         <v>310</v>
       </c>
       <c r="J25" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2585</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-437</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-1654</v>
       </c>
-      <c r="N25" s="7">
-        <f>SUM(N23:N24)</f>
+      <c r="M25" s="10">
+        <f t="shared" ref="M25" si="15">SUM(M23:M24)</f>
+        <v>-16989</v>
+      </c>
+      <c r="P25" s="7">
+        <f>SUM(P23:P24)</f>
         <v>21221</v>
       </c>
-      <c r="O25" s="7">
-        <f t="shared" ref="O25:P25" si="11">SUM(O23:O24)</f>
+      <c r="Q25" s="7">
+        <f t="shared" ref="Q25:R25" si="16">SUM(Q23:Q24)</f>
         <v>8017</v>
       </c>
-      <c r="P25" s="7">
-        <f t="shared" si="11"/>
+      <c r="R25" s="7">
+        <f t="shared" si="16"/>
         <v>1675</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="P27">
+        <v>29456</v>
+      </c>
+      <c r="Q27">
+        <v>15433</v>
+      </c>
+      <c r="R27">
+        <v>11471</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="P28" s="6">
+        <f>-18733-1598</f>
+        <v>-20331</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>-24844-206</f>
+        <v>-25050</v>
+      </c>
+      <c r="R28" s="6">
+        <f>-18733-1596</f>
+        <v>-20329</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="P29">
+        <f>SUM(P27:P28)</f>
+        <v>9125</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ref="Q29:R29" si="17">SUM(Q27:Q28)</f>
+        <v>-9617</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="17"/>
+        <v>-8858</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8">
-        <f t="shared" ref="H27:L27" si="12">H13/G13-1</f>
-        <v>0.10533504054630805</v>
-      </c>
-      <c r="I27" s="8">
-        <f t="shared" si="12"/>
-        <v>9.3366283110664972E-2</v>
-      </c>
-      <c r="J27" s="8">
-        <f t="shared" si="12"/>
-        <v>8.8148043508970098E-2</v>
-      </c>
-      <c r="K27" s="8">
-        <f t="shared" si="12"/>
-        <v>-0.17408801765545889</v>
-      </c>
-      <c r="L27" s="8">
-        <f t="shared" si="12"/>
-        <v>8.5664885256209189E-3</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8">
-        <f>O13/N13-1</f>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8">
+        <f>K13/G13-1</f>
+        <v>8.6128894579598825E-2</v>
+      </c>
+      <c r="L33" s="8">
+        <f t="shared" ref="L33:M33" si="18">L13/H13-1</f>
+        <v>-8.9582207120241231E-3</v>
+      </c>
+      <c r="M33" s="8">
+        <f t="shared" si="18"/>
+        <v>-6.1731883034326862E-2</v>
+      </c>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8">
+        <f>Q13/P13-1</f>
         <v>-0.20209050415063778</v>
       </c>
-      <c r="P27" s="8">
-        <f>P13/O13-1</f>
+      <c r="R33" s="8">
+        <f>R13/Q13-1</f>
         <v>-0.13997525930155108</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>115</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8">
-        <f t="shared" ref="H28:L28" si="13">H15/G15-1</f>
-        <v>0.15718562874251507</v>
-      </c>
-      <c r="I28" s="8">
-        <f t="shared" si="13"/>
-        <v>0.29754204398447603</v>
-      </c>
-      <c r="J28" s="8">
-        <f t="shared" si="13"/>
-        <v>0.17098703888334987</v>
-      </c>
-      <c r="K28" s="8">
-        <f t="shared" si="13"/>
-        <v>-0.25968497232865051</v>
-      </c>
-      <c r="L28" s="8">
-        <f t="shared" si="13"/>
-        <v>-0.12842629863906463</v>
-      </c>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8">
-        <f>O15/N15-1</f>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8">
+        <f>K15/G15-1</f>
+        <v>0.30164670658682624</v>
+      </c>
+      <c r="L34" s="8">
+        <f t="shared" ref="L34:M34" si="19">L15/H15-1</f>
+        <v>-1.9620526088831358E-2</v>
+      </c>
+      <c r="M34" s="8">
+        <f t="shared" si="19"/>
+        <v>-0.66816218012628781</v>
+      </c>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8">
+        <f>Q15/P15-1</f>
         <v>-0.38683099395184295</v>
       </c>
-      <c r="P28" s="8">
-        <f>P15/O15-1</f>
+      <c r="R34" s="8">
+        <f>R15/Q15-1</f>
         <v>-0.19187821037742869</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8">
-        <f t="shared" ref="H29:L29" si="14">H20/G20-1</f>
-        <v>-0.30790190735694822</v>
-      </c>
-      <c r="I29" s="8">
-        <f t="shared" si="14"/>
-        <v>-0.99212598425196852</v>
-      </c>
-      <c r="J29" s="8">
-        <f t="shared" si="14"/>
-        <v>-324.125</v>
-      </c>
-      <c r="K29" s="8">
-        <f t="shared" si="14"/>
-        <v>-1.4135396518375241</v>
-      </c>
-      <c r="L29" s="8">
-        <f t="shared" si="14"/>
-        <v>0.83723105706267531</v>
-      </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8">
-        <f>O20/N20-1</f>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8">
+        <f>(K20-G20)/ABS(G20)</f>
+        <v>0.27179836512261579</v>
+      </c>
+      <c r="L35" s="8">
+        <f t="shared" ref="L35:M35" si="20">(L20-H20)/ABS(H20)</f>
+        <v>-0.93307086614173229</v>
+      </c>
+      <c r="M35" s="8">
+        <f t="shared" si="20"/>
+        <v>-1131.125</v>
+      </c>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8">
+        <f>Q20/P20-1</f>
         <v>-0.88003700657894735</v>
       </c>
-      <c r="P29" s="8">
-        <f>P20/O20-1</f>
+      <c r="R35" s="8">
+        <f>R20/Q20-1</f>
         <v>-0.96015424164524421</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="8">
-        <f t="shared" ref="G30:L30" si="15">G16/G19</f>
+      <c r="G36" s="8">
+        <f t="shared" ref="G36:L36" si="21">G16/G19</f>
         <v>0.75036523009495981</v>
       </c>
-      <c r="H30" s="8">
-        <f t="shared" si="15"/>
+      <c r="H36" s="8">
+        <f t="shared" si="21"/>
         <v>0.72161301733286165</v>
       </c>
-      <c r="I30" s="8">
-        <f t="shared" si="15"/>
+      <c r="I36" s="8">
+        <f t="shared" si="21"/>
         <v>0.64221705940922669</v>
       </c>
-      <c r="J30" s="8">
-        <f t="shared" si="15"/>
+      <c r="J36" s="8">
+        <f t="shared" si="21"/>
         <v>0.89354549529359029</v>
       </c>
-      <c r="K30" s="8">
-        <f t="shared" si="15"/>
+      <c r="K36" s="8">
+        <f t="shared" si="21"/>
         <v>0.69710467706013368</v>
       </c>
-      <c r="L30" s="8">
-        <f t="shared" si="15"/>
+      <c r="L36" s="8">
+        <f t="shared" si="21"/>
         <v>0.65105206573491015</v>
       </c>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8">
-        <f>N16/N19</f>
+      <c r="M36" s="8">
+        <f t="shared" ref="M36" si="22">M16/M19</f>
+        <v>0.3662927447077981</v>
+      </c>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8">
+        <f>P16/P19</f>
         <v>0.62358881727492921</v>
       </c>
-      <c r="O30" s="8">
-        <f t="shared" ref="O30:P30" si="16">O16/O19</f>
+      <c r="Q36" s="8">
+        <f t="shared" ref="Q36:R36" si="23">Q16/Q19</f>
         <v>0.71449535300831568</v>
       </c>
-      <c r="P30" s="8">
-        <f t="shared" si="16"/>
+      <c r="R36" s="8">
+        <f t="shared" si="23"/>
         <v>0.74225182718105287</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>119</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8">
-        <f t="shared" ref="H31:L31" si="17">H16/G16-1</f>
-        <v>-7.0576782672182592E-3</v>
-      </c>
-      <c r="I31" s="8">
-        <f t="shared" si="17"/>
-        <v>-5.1470588235294157E-2</v>
-      </c>
-      <c r="J31" s="8">
-        <f t="shared" si="17"/>
-        <v>3.0232558139534849E-2</v>
-      </c>
-      <c r="K31" s="8">
-        <f t="shared" si="17"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8">
+        <f t="shared" ref="K37:M37" si="24">K16/J16-1</f>
         <v>9.9071983947830455E-2</v>
       </c>
-      <c r="L31" s="8">
-        <f t="shared" si="17"/>
+      <c r="L37" s="8">
+        <f t="shared" si="24"/>
         <v>-3.2633500684618899E-2</v>
       </c>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8">
-        <f>O16/N16-1</f>
+      <c r="M37" s="8">
+        <f t="shared" si="24"/>
+        <v>-4.4821891955649895E-2</v>
+      </c>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8">
+        <f>Q16/P16-1</f>
         <v>0.15391705069124417</v>
       </c>
-      <c r="P31" s="8">
-        <f>P16/O16-1</f>
+      <c r="R37" s="8">
+        <f>R16/Q16-1</f>
         <v>-8.4550433591967122E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8">
-        <f t="shared" ref="H32:L32" si="18">H25/G25-1</f>
-        <v>-1.5321531791907514</v>
-      </c>
-      <c r="I32" s="8">
-        <f t="shared" si="18"/>
-        <v>-0.78954514596062464</v>
-      </c>
-      <c r="J32" s="8">
-        <f t="shared" si="18"/>
-        <v>7.3387096774193541</v>
-      </c>
-      <c r="K32" s="8">
-        <f t="shared" si="18"/>
-        <v>-1.1690522243713732</v>
-      </c>
-      <c r="L32" s="8">
-        <f t="shared" si="18"/>
-        <v>2.7848970251716247</v>
-      </c>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8">
-        <f>O25/N25-1</f>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8">
+        <f>(K25-G25)/ABS(G25)</f>
+        <v>0.84212427745664742</v>
+      </c>
+      <c r="L38" s="8">
+        <f>(L25-H25)/ABS(H25)</f>
+        <v>-2.1228784792939579</v>
+      </c>
+      <c r="M38" s="8">
+        <f>(M25-I25)/ABS(I25)</f>
+        <v>-55.803225806451614</v>
+      </c>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8">
+        <f>Q25/P25-1</f>
         <v>-0.62221384477640074</v>
       </c>
-      <c r="P32" s="8">
-        <f>P25/O25-1</f>
+      <c r="R38" s="8">
+        <f>R25/Q25-1</f>
         <v>-0.79106897842085566</v>
       </c>
     </row>

</xml_diff>